<commit_message>
fixed move out data
</commit_message>
<xml_diff>
--- a/tools/baidu-qianxi/move_out/七台河.xlsx
+++ b/tools/baidu-qianxi/move_out/七台河.xlsx
@@ -35,7 +35,6 @@
     <sheet name="20200204" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="20200205" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="20200206" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="20200207" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -35210,42 +35209,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>城市</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>省份</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>比例</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>